<commit_message>
coordinate colors fig 1 and 2
try to coordinate colors - did not succeed
some issue with the map code - ask PMR
* archive of ms version submitted to coauthors
</commit_message>
<xml_diff>
--- a/figures/data-raw/2003_2005_capelin_version1.xlsx
+++ b/figures/data-raw/2003_2005_capelin_version1.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9303"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\murphyh\Documents\Documents\Capelin\Response to Frank et al. 2016\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="15585" yWindow="-15" windowWidth="10155" windowHeight="11760" activeTab="2"/>
+    <workbookView xWindow="15585" yWindow="-15" windowWidth="10155" windowHeight="11760" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Mat_Imm_Spent" sheetId="10" r:id="rId1"/>
@@ -12,12 +17,12 @@
     <sheet name="Biomass_2003_2005" sheetId="12" r:id="rId3"/>
     <sheet name="Larval_densities" sheetId="13" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="145621"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="65" uniqueCount="43">
   <si>
     <t>Oct</t>
   </si>
@@ -28,6 +33,9 @@
     <t>Jun</t>
   </si>
   <si>
+    <t xml:space="preserve">Jan </t>
+  </si>
+  <si>
     <t>Trip</t>
   </si>
   <si>
@@ -97,15 +105,33 @@
     <t>Mean_dens</t>
   </si>
   <si>
+    <t>Mean length</t>
+  </si>
+  <si>
+    <t>mean weight</t>
+  </si>
+  <si>
     <t>TS</t>
   </si>
   <si>
     <t>crosssection</t>
   </si>
   <si>
+    <t>survey area km2</t>
+  </si>
+  <si>
+    <t>abundance (millions</t>
+  </si>
+  <si>
+    <t>biomass (kg)</t>
+  </si>
+  <si>
     <t>billions</t>
   </si>
   <si>
+    <t>biomass (kilotonnes)</t>
+  </si>
+  <si>
     <t>Tel</t>
   </si>
   <si>
@@ -121,28 +147,16 @@
     <t>Year_2000</t>
   </si>
   <si>
-    <t>Meanlength</t>
-  </si>
-  <si>
-    <t>meanweight</t>
-  </si>
-  <si>
-    <t>surveyareakm2</t>
-  </si>
-  <si>
-    <t>abundance(millions</t>
-  </si>
-  <si>
-    <t>biomass(kg)</t>
-  </si>
-  <si>
-    <t>biomass(kilotonnes)</t>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>SE</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="0.0"/>
@@ -200,173 +214,6 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <c:date1904 val="0"/>
-  <c:lang val="en-CA"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:invertIfNegative val="0"/>
-          <c:val>
-            <c:numRef>
-              <c:f>Biomass_2003_2005!$K$2:$K$12</c:f>
-              <c:numCache>
-                <c:formatCode>0.0000</c:formatCode>
-                <c:ptCount val="11"/>
-                <c:pt idx="0">
-                  <c:v>24.73</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>54.45982878170858</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>13.09064650819086</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>13.159803046976643</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>10.4</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>10966.589907201134</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>880.08285081843712</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>11.837259073137954</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>111.3</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13702.974929707392</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.4054150292725682</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-        </c:ser>
-        <c:dLbls>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="150"/>
-        <c:axId val="82165760"/>
-        <c:axId val="82167296"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="82165760"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82167296"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="82167296"/>
-        <c:scaling>
-          <c:logBase val="10"/>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines/>
-        <c:numFmt formatCode="0.0000" sourceLinked="1"/>
-        <c:majorTickMark val="out"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:crossAx val="82165760"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-    </c:plotArea>
-    <c:legend>
-      <c:legendPos val="r"/>
-      <c:layout/>
-      <c:overlay val="0"/>
-    </c:legend>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>10</xdr:col>
-      <xdr:colOff>247650</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>142875</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>314325</xdr:colOff>
-      <xdr:row>29</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="2" name="Chart 1"/>
-        <xdr:cNvGraphicFramePr/>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
@@ -410,7 +257,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -445,7 +292,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -667,28 +514,28 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C1" t="s">
+        <v>18</v>
+      </c>
+      <c r="D1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
+        <v>19</v>
+      </c>
+      <c r="F1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G1" t="s">
+        <v>20</v>
+      </c>
+      <c r="H1" t="s">
         <v>7</v>
-      </c>
-      <c r="E1" t="s">
-        <v>18</v>
-      </c>
-      <c r="F1" t="s">
-        <v>9</v>
-      </c>
-      <c r="G1" t="s">
-        <v>19</v>
-      </c>
-      <c r="H1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
@@ -721,7 +568,7 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>566</v>
@@ -778,7 +625,7 @@
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>115</v>
@@ -836,7 +683,7 @@
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <v>2965</v>
@@ -864,7 +711,7 @@
   <dimension ref="A1:L7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="L13" sqref="L13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -876,40 +723,40 @@
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="C1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="D1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="E1" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="F1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="H1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="I1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="J1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="L1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.25">
@@ -957,7 +804,7 @@
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B3" s="1">
         <v>61</v>
@@ -1042,7 +889,7 @@
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B5" s="1">
         <v>21</v>
@@ -1126,7 +973,7 @@
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B7" s="1">
         <f>SUM(B2:B6)</f>
@@ -1165,79 +1012,71 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:P12"/>
+  <dimension ref="A1:M12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D23" sqref="D23"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="12.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.140625" customWidth="1"/>
     <col min="9" max="10" width="13.5703125" customWidth="1"/>
-    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="19.85546875" customWidth="1"/>
     <col min="12" max="12" width="16.140625" customWidth="1"/>
     <col min="13" max="13" width="13.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C1" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G1" t="s">
+        <v>29</v>
+      </c>
+      <c r="H1" t="s">
+        <v>30</v>
+      </c>
+      <c r="I1" t="s">
+        <v>31</v>
+      </c>
+      <c r="J1" t="s">
+        <v>32</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
         <v>34</v>
       </c>
-      <c r="F1" t="s">
+      <c r="M1" s="2" t="s">
         <v>35</v>
       </c>
-      <c r="G1" t="s">
-        <v>26</v>
-      </c>
-      <c r="H1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I1" t="s">
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>36</v>
-      </c>
-      <c r="J1" t="s">
-        <v>37</v>
-      </c>
-      <c r="K1" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="L1" t="s">
-        <v>28</v>
-      </c>
-      <c r="M1" s="2" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>29</v>
       </c>
       <c r="B2">
         <v>2003</v>
       </c>
       <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="I2">
-        <v>2073</v>
+        <v>12</v>
       </c>
       <c r="J2">
         <v>2.88</v>
@@ -1246,12 +1085,8 @@
         <v>24.73</v>
       </c>
       <c r="M2" s="2"/>
-      <c r="P2">
-        <f>+K2/I2</f>
-        <v>1.1929570670525809E-2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>502</v>
       </c>
@@ -1259,7 +1094,7 @@
         <v>2003</v>
       </c>
       <c r="C3" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D3" s="3">
         <v>1.1600000000000001E-7</v>
@@ -1275,7 +1110,7 @@
         <v>-52.285316715792675</v>
       </c>
       <c r="H3" s="1">
-        <f>+POWER(10,((20*LOG(E3)-67.5)/10))</f>
+        <f>+POWER(10,((20*LOG(E3) - 67.5)/10))</f>
         <v>2.1452026679753134E-5</v>
       </c>
       <c r="I3">
@@ -1297,12 +1132,8 @@
         <f>K3/1000</f>
         <v>5.4459828781708582E-2</v>
       </c>
-      <c r="P3">
-        <f>+K3/I3</f>
-        <v>2.627102208476053E-2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>504</v>
       </c>
@@ -1326,14 +1157,14 @@
         <v>-51.626778359946485</v>
       </c>
       <c r="H4" s="1">
-        <f>+POWER(10,((20*LOG(E4)-67.5)/10))</f>
+        <f t="shared" ref="H4:H12" si="1">+POWER(10,((20*LOG(E4) - 67.5)/10))</f>
         <v>2.4964459288828971E-5</v>
       </c>
       <c r="I4">
         <v>2073</v>
       </c>
       <c r="J4" s="3">
-        <f t="shared" ref="J4:J12" si="1">D4/H4*I4</f>
+        <f t="shared" ref="J4:J12" si="2">D4/H4*I4</f>
         <v>2.0344322066982121</v>
       </c>
       <c r="K4" s="2">
@@ -1341,19 +1172,15 @@
         <v>13.09064650819086</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" ref="L4:M12" si="2">J4/1000</f>
+        <f t="shared" ref="L4:M12" si="3">J4/1000</f>
         <v>2.034432206698212E-3</v>
       </c>
       <c r="M4" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.309064650819086E-2</v>
       </c>
-      <c r="P4">
-        <f t="shared" ref="P4:P12" si="3">+K4/I4</f>
-        <v>6.3148318901065413E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>512</v>
       </c>
@@ -1377,14 +1204,14 @@
         <v>-56.302309310504214</v>
       </c>
       <c r="H5" s="1">
-        <f>+POWER(10,((20*LOG(E5)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>8.506855757351828E-6</v>
       </c>
       <c r="I5">
         <v>2073</v>
       </c>
       <c r="J5" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>7.1643626903311288</v>
       </c>
       <c r="K5" s="2">
@@ -1392,27 +1219,23 @@
         <v>13.159803046976643</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>7.1643626903311287E-3</v>
       </c>
       <c r="M5" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3159803046976642E-2</v>
       </c>
-      <c r="P5">
-        <f t="shared" si="3"/>
-        <v>6.3481924973355728E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B6">
         <v>2004</v>
       </c>
       <c r="C6" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="3"/>
       <c r="F6" s="1"/>
@@ -1427,7 +1250,7 @@
       <c r="L6" s="3"/>
       <c r="M6" s="2"/>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>565</v>
       </c>
@@ -1451,14 +1274,14 @@
         <v>-52.018874522335167</v>
       </c>
       <c r="H7" s="1">
-        <f>+POWER(10,((20*LOG(E7)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>2.2809331010735011E-5</v>
       </c>
       <c r="I7">
         <v>2073</v>
       </c>
       <c r="J7" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>1108.7830672498551</v>
       </c>
       <c r="K7" s="2">
@@ -1466,19 +1289,15 @@
         <v>10966.589907201134</v>
       </c>
       <c r="L7" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1087830672498551</v>
       </c>
       <c r="M7" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>10.966589907201135</v>
       </c>
-      <c r="P7">
-        <f t="shared" si="3"/>
-        <v>5.2902025601549125</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>573</v>
       </c>
@@ -1486,7 +1305,7 @@
         <v>2004</v>
       </c>
       <c r="C8" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D8" s="3">
         <v>1.1599999999999999E-6</v>
@@ -1502,14 +1321,14 @@
         <v>-49.977840110858672</v>
       </c>
       <c r="H8" s="1">
-        <f>+POWER(10,((20*LOG(E8)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>3.6493539616360884E-5</v>
       </c>
       <c r="I8">
         <v>2073</v>
       </c>
       <c r="J8" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>65.893306740843713</v>
       </c>
       <c r="K8" s="2">
@@ -1517,19 +1336,15 @@
         <v>880.08285081843712</v>
       </c>
       <c r="L8" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>6.5893306740843718E-2</v>
       </c>
       <c r="M8" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.88008285081843707</v>
       </c>
-      <c r="P8">
-        <f t="shared" si="3"/>
-        <v>0.42454551414299907</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>581</v>
       </c>
@@ -1537,7 +1352,7 @@
         <v>2005</v>
       </c>
       <c r="C9" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="D9" s="3">
         <v>1.6700000000000001E-8</v>
@@ -1553,14 +1368,14 @@
         <v>-49.900539464197635</v>
       </c>
       <c r="H9" s="1">
-        <f>+POWER(10,((20*LOG(E9)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>3.7148908126090031E-5</v>
       </c>
       <c r="I9">
         <v>2073</v>
       </c>
       <c r="J9" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>0.93190087532308064</v>
       </c>
       <c r="K9" s="2">
@@ -1568,27 +1383,23 @@
         <v>11.837259073137954</v>
       </c>
       <c r="L9" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9.3190087532308067E-4</v>
       </c>
       <c r="M9" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.1837259073137953E-2</v>
       </c>
-      <c r="P9">
-        <f t="shared" si="3"/>
-        <v>5.7102069817356266E-3</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="B10">
         <v>2005</v>
       </c>
       <c r="C10" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="3"/>
       <c r="F10" s="1"/>
@@ -1603,7 +1414,7 @@
       <c r="L10" s="3"/>
       <c r="M10" s="2"/>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>639</v>
       </c>
@@ -1627,14 +1438,14 @@
         <v>-50.583417550803205</v>
       </c>
       <c r="H11" s="1">
-        <f>+POWER(10,((20*LOG(E11)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>3.1743751077898298E-5</v>
       </c>
       <c r="I11">
         <v>2073</v>
       </c>
       <c r="J11" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>979.56287282160577</v>
       </c>
       <c r="K11" s="2">
@@ -1642,19 +1453,15 @@
         <v>13702.974929707392</v>
       </c>
       <c r="L11" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>0.97956287282160581</v>
       </c>
       <c r="M11" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13.702974929707393</v>
       </c>
-      <c r="P11">
-        <f t="shared" si="3"/>
-        <v>6.6102146308284571</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>647</v>
       </c>
@@ -1662,7 +1469,7 @@
         <v>2005</v>
       </c>
       <c r="C12" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="D12" s="3">
         <v>9.3299999999999998E-9</v>
@@ -1678,14 +1485,14 @@
         <v>-64.008019805134069</v>
       </c>
       <c r="H12" s="1">
-        <f>+POWER(10,((20*LOG(E12)-67.5)/10))</f>
+        <f t="shared" si="1"/>
         <v>1.4427730436356264E-6</v>
       </c>
       <c r="I12">
         <v>2073</v>
       </c>
       <c r="J12" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>13.405497202292205</v>
       </c>
       <c r="K12" s="2">
@@ -1693,30 +1500,25 @@
         <v>1.4054150292725682</v>
       </c>
       <c r="L12" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.3405497202292204E-2</v>
       </c>
       <c r="M12" s="2">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1.4054150292725682E-3</v>
-      </c>
-      <c r="P12">
-        <f t="shared" si="3"/>
-        <v>6.7796190510012943E-4</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D16"/>
+  <dimension ref="A1:F16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1724,24 +1526,30 @@
     <col min="1" max="1" width="11.7109375" customWidth="1"/>
     <col min="2" max="2" width="12.85546875" customWidth="1"/>
     <col min="3" max="3" width="11.140625" style="5" customWidth="1"/>
-    <col min="4" max="4" width="8" customWidth="1"/>
+    <col min="4" max="4" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>32</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>30</v>
+        <v>37</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>33</v>
+        <v>40</v>
       </c>
       <c r="D1" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+      <c r="E1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1982</v>
       </c>
@@ -1754,8 +1562,14 @@
       <c r="D2" s="4">
         <v>23.15546217</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>13.020044338958821</v>
+      </c>
+      <c r="F2">
+        <v>5.3154108431436367</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1983</v>
       </c>
@@ -1766,10 +1580,16 @@
         <v>2003</v>
       </c>
       <c r="D3" s="4">
-        <v>48.069988219999999</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>52.882950682132957</v>
+      </c>
+      <c r="E3">
+        <v>32.918789551720266</v>
+      </c>
+      <c r="F3">
+        <v>7.5520882631384847</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1984</v>
       </c>
@@ -1782,8 +1602,14 @@
       <c r="D4" s="4">
         <v>14.864253140000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>10.952753383945588</v>
+      </c>
+      <c r="F4">
+        <v>2.5127339554811554</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1985</v>
       </c>
@@ -1796,8 +1622,14 @@
       <c r="D5" s="4">
         <v>9.9197824089999997</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E5">
+        <v>14.249068433834005</v>
+      </c>
+      <c r="F5">
+        <v>3.2689604917198842</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1986</v>
       </c>
@@ -1810,80 +1642,140 @@
       <c r="D6" s="4">
         <v>18.22882491</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E6">
+        <v>13.832118461893558</v>
+      </c>
+      <c r="F6">
+        <v>3.2602615875268577</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C7" s="5">
         <v>2007</v>
       </c>
       <c r="D7" s="4">
         <v>75.49157538</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E7">
+        <v>34.36583775716452</v>
+      </c>
+      <c r="F7">
+        <v>7.8840638891365584</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C8" s="5">
         <v>2008</v>
       </c>
       <c r="D8" s="4">
         <v>48.547551919999997</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8">
+        <v>38.885083203626849</v>
+      </c>
+      <c r="F8">
+        <v>8.9208498997779078</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C9" s="5">
         <v>2009</v>
       </c>
       <c r="D9" s="4">
         <v>12.65858671</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9">
+        <v>6.3573299086900823</v>
+      </c>
+      <c r="F9">
+        <v>1.4584715064594065</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C10" s="5">
         <v>2010</v>
       </c>
       <c r="D10" s="4">
         <v>26.38670677</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10">
+        <v>25.4060048504153</v>
+      </c>
+      <c r="F10">
+        <v>5.8285372474770769</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C11" s="5">
         <v>2011</v>
       </c>
       <c r="D11" s="4">
         <v>96.955608650000002</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11">
+        <v>98.802940058063982</v>
+      </c>
+      <c r="F11">
+        <v>22.66694900198987</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C12" s="5">
         <v>2012</v>
       </c>
       <c r="D12" s="4">
         <v>9.8337581600000004</v>
       </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E12">
+        <v>12.44497121049063</v>
+      </c>
+      <c r="F12">
+        <v>3.45161398623824</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C13" s="5">
         <v>2013</v>
       </c>
       <c r="D13" s="4">
         <v>12.76704148</v>
       </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E13">
+        <v>8.6632332137421173</v>
+      </c>
+      <c r="F13">
+        <v>2.0419436508125264</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C14" s="5">
         <v>2014</v>
       </c>
       <c r="D14" s="4">
         <v>25.510123230000001</v>
       </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E14">
+        <v>13.893954452450302</v>
+      </c>
+      <c r="F14">
+        <v>3.1874917570730448</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="C15" s="5">
         <v>2015</v>
       </c>
       <c r="D15" s="4">
         <v>9.7228972299999992</v>
       </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E15">
+        <v>11.043119825126364</v>
+      </c>
+      <c r="F15">
+        <v>2.5334654389019144</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="D16" s="4"/>
     </row>
   </sheetData>

</xml_diff>